<commit_message>
Soem updates are done in Test Data sheet.
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -1967,10 +1967,10 @@
   <dimension ref="A1:CG281"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D136" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F167" sqref="F167"/>
+      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Latest clinique changes under source file.
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="448">
   <si>
     <t>Ankit</t>
   </si>
@@ -1354,6 +1354,12 @@
   </si>
   <si>
     <t>SS_ItemDelete_OneItem_CheckOut</t>
+  </si>
+  <si>
+    <t>SS_CheckOut_NewAddress_Clinique</t>
+  </si>
+  <si>
+    <t>BRANDS</t>
   </si>
 </sst>
 </file>
@@ -1976,13 +1982,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG281"/>
+  <dimension ref="A1:CG282"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B161" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D182" sqref="D182"/>
+      <selection pane="bottomRight" activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13589,7 +13595,7 @@
     </row>
     <row r="116" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>125</v>
+        <v>446</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>367</v>
@@ -13603,10 +13609,10 @@
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="2" t="s">
-        <v>53</v>
+        <v>447</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>327</v>
+        <v>6</v>
       </c>
       <c r="I116" s="1"/>
       <c r="J116" s="2" t="s">
@@ -13664,21 +13670,12 @@
       <c r="AX116" s="1"/>
       <c r="AY116" s="1"/>
       <c r="AZ116" s="1"/>
-      <c r="BA116" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB116" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BD116" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BE116" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF116" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="BA116" s="1"/>
+      <c r="BB116" s="1"/>
+      <c r="BC116" s="1"/>
+      <c r="BD116" s="1"/>
+      <c r="BE116" s="1"/>
+      <c r="BF116" s="1"/>
       <c r="BG116" s="1"/>
       <c r="BH116" s="1"/>
       <c r="BI116" s="1"/>
@@ -13706,12 +13703,12 @@
       <c r="CE116" s="1"/>
       <c r="CF116" s="1"/>
       <c r="CG116" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="117" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>367</v>
@@ -13787,18 +13784,21 @@
       <c r="AY117" s="1"/>
       <c r="AZ117" s="1"/>
       <c r="BA117" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BB117" s="1"/>
-      <c r="BC117" s="1"/>
-      <c r="BD117" s="1"/>
-      <c r="BE117" s="1"/>
-      <c r="BF117" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="BG117" s="4" t="s">
-        <v>133</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="BB117" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD117" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE117" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF117" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="BG117" s="1"/>
       <c r="BH117" s="1"/>
       <c r="BI117" s="1"/>
       <c r="BJ117" s="1"/>
@@ -13830,7 +13830,7 @@
     </row>
     <row r="118" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>396</v>
+        <v>131</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>367</v>
@@ -13944,12 +13944,12 @@
       <c r="CE118" s="1"/>
       <c r="CF118" s="1"/>
       <c r="CG118" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="119" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>367</v>
@@ -14011,12 +14011,8 @@
       <c r="AK119" s="1"/>
       <c r="AL119" s="1"/>
       <c r="AM119" s="1"/>
-      <c r="AN119" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="AO119" s="1" t="s">
-        <v>399</v>
-      </c>
+      <c r="AN119" s="1"/>
+      <c r="AO119" s="1"/>
       <c r="AP119" s="1"/>
       <c r="AQ119" s="1"/>
       <c r="AR119" s="1"/>
@@ -14045,14 +14041,10 @@
       <c r="BI119" s="1"/>
       <c r="BJ119" s="1"/>
       <c r="BK119" s="1"/>
-      <c r="BL119" s="1" t="s">
-        <v>441</v>
-      </c>
+      <c r="BL119" s="1"/>
       <c r="BM119" s="1"/>
       <c r="BN119" s="1"/>
-      <c r="BO119" s="1" t="s">
-        <v>402</v>
-      </c>
+      <c r="BO119" s="1"/>
       <c r="BP119" s="1"/>
       <c r="BQ119" s="1"/>
       <c r="BR119" s="1"/>
@@ -14076,7 +14068,7 @@
     </row>
     <row r="120" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>367</v>
@@ -14203,16 +14195,16 @@
     </row>
     <row r="121" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>431</v>
+        <v>2</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>364</v>
+        <v>3</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -14330,7 +14322,7 @@
     </row>
     <row r="122" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>367</v>
@@ -14347,7 +14339,7 @@
         <v>53</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>418</v>
+        <v>327</v>
       </c>
       <c r="I122" s="1"/>
       <c r="J122" s="2" t="s">
@@ -14452,12 +14444,12 @@
       <c r="CE122" s="1"/>
       <c r="CF122" s="1"/>
       <c r="CG122" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="123" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>367</v>
@@ -14474,7 +14466,7 @@
         <v>53</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>327</v>
+        <v>418</v>
       </c>
       <c r="I123" s="1"/>
       <c r="J123" s="2" t="s">
@@ -14579,12 +14571,12 @@
       <c r="CE123" s="1"/>
       <c r="CF123" s="1"/>
       <c r="CG123" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="124" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>367</v>
@@ -14711,7 +14703,7 @@
     </row>
     <row r="125" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>367</v>
@@ -14838,16 +14830,16 @@
     </row>
     <row r="126" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>2</v>
+        <v>431</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>3</v>
+        <v>364</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -14965,7 +14957,7 @@
     </row>
     <row r="127" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>367</v>
@@ -15092,7 +15084,7 @@
     </row>
     <row r="128" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>367</v>
@@ -15147,10 +15139,9 @@
       <c r="AD128" s="1"/>
       <c r="AE128" s="1"/>
       <c r="AF128" s="1"/>
-      <c r="AG128" s="1">
-        <v>324353454</v>
-      </c>
+      <c r="AG128" s="1"/>
       <c r="AH128" s="1"/>
+      <c r="AI128" s="1"/>
       <c r="AJ128" s="1"/>
       <c r="AK128" s="1"/>
       <c r="AL128" s="1"/>
@@ -15220,7 +15211,7 @@
     </row>
     <row r="129" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>367</v>
@@ -15275,11 +15266,10 @@
       <c r="AD129" s="1"/>
       <c r="AE129" s="1"/>
       <c r="AF129" s="1"/>
-      <c r="AG129" s="1"/>
+      <c r="AG129" s="1">
+        <v>324353454</v>
+      </c>
       <c r="AH129" s="1"/>
-      <c r="AI129" s="1" t="s">
-        <v>429</v>
-      </c>
       <c r="AJ129" s="1"/>
       <c r="AK129" s="1"/>
       <c r="AL129" s="1"/>
@@ -15344,12 +15334,12 @@
       <c r="CE129" s="1"/>
       <c r="CF129" s="1"/>
       <c r="CG129" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="130" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>367</v>
@@ -15406,13 +15396,13 @@
       <c r="AF130" s="1"/>
       <c r="AG130" s="1"/>
       <c r="AH130" s="1"/>
-      <c r="AI130" s="1"/>
+      <c r="AI130" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="AJ130" s="1"/>
       <c r="AK130" s="1"/>
       <c r="AL130" s="1"/>
-      <c r="AM130" s="26" t="s">
-        <v>428</v>
-      </c>
+      <c r="AM130" s="1"/>
       <c r="AN130" s="1" t="s">
         <v>398</v>
       </c>
@@ -15473,12 +15463,12 @@
       <c r="CE130" s="1"/>
       <c r="CF130" s="1"/>
       <c r="CG130" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="131" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>367</v>
@@ -15537,11 +15527,11 @@
       <c r="AH131" s="1"/>
       <c r="AI131" s="1"/>
       <c r="AJ131" s="1"/>
-      <c r="AK131" s="1" t="s">
-        <v>427</v>
-      </c>
+      <c r="AK131" s="1"/>
       <c r="AL131" s="1"/>
-      <c r="AM131" s="1"/>
+      <c r="AM131" s="26" t="s">
+        <v>428</v>
+      </c>
       <c r="AN131" s="1" t="s">
         <v>398</v>
       </c>
@@ -15607,7 +15597,7 @@
     </row>
     <row r="132" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>367</v>
@@ -15666,7 +15656,9 @@
       <c r="AH132" s="1"/>
       <c r="AI132" s="1"/>
       <c r="AJ132" s="1"/>
-      <c r="AK132" s="1"/>
+      <c r="AK132" s="1" t="s">
+        <v>427</v>
+      </c>
       <c r="AL132" s="1"/>
       <c r="AM132" s="1"/>
       <c r="AN132" s="1" t="s">
@@ -15734,7 +15726,7 @@
     </row>
     <row r="133" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>367</v>
@@ -15861,7 +15853,7 @@
     </row>
     <row r="134" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>367</v>
@@ -15988,16 +15980,16 @@
     </row>
     <row r="135" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>407</v>
+        <v>426</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>431</v>
+        <v>2</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>364</v>
+        <v>3</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -16115,7 +16107,7 @@
     </row>
     <row r="136" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>367</v>
@@ -16242,7 +16234,7 @@
     </row>
     <row r="137" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>367</v>
@@ -16369,7 +16361,7 @@
     </row>
     <row r="138" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>430</v>
+        <v>408</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>367</v>
@@ -16496,16 +16488,16 @@
     </row>
     <row r="139" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>409</v>
+        <v>430</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>2</v>
+        <v>431</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>3</v>
+        <v>364</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -16623,13 +16615,13 @@
     </row>
     <row r="140" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C140" s="26" t="s">
-        <v>411</v>
+      <c r="C140" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>3</v>
@@ -16750,7 +16742,7 @@
     </row>
     <row r="141" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>367</v>
@@ -16767,7 +16759,7 @@
         <v>53</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>418</v>
+        <v>327</v>
       </c>
       <c r="I141" s="1"/>
       <c r="J141" s="2" t="s">
@@ -16872,18 +16864,18 @@
       <c r="CE141" s="1"/>
       <c r="CF141" s="1"/>
       <c r="CG141" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="142" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>2</v>
+      <c r="C142" s="26" t="s">
+        <v>411</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>3</v>
@@ -16894,7 +16886,7 @@
         <v>53</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>327</v>
+        <v>418</v>
       </c>
       <c r="I142" s="1"/>
       <c r="J142" s="2" t="s">
@@ -16999,12 +16991,12 @@
       <c r="CE142" s="1"/>
       <c r="CF142" s="1"/>
       <c r="CG142" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="143" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>367</v>
@@ -17131,7 +17123,7 @@
     </row>
     <row r="144" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>135</v>
+        <v>401</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>367</v>
@@ -17193,8 +17185,12 @@
       <c r="AK144" s="1"/>
       <c r="AL144" s="1"/>
       <c r="AM144" s="1"/>
-      <c r="AN144" s="1"/>
-      <c r="AO144" s="1"/>
+      <c r="AN144" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="AO144" s="1" t="s">
+        <v>399</v>
+      </c>
       <c r="AP144" s="1"/>
       <c r="AQ144" s="1"/>
       <c r="AR144" s="1"/>
@@ -17207,30 +17203,30 @@
       <c r="AY144" s="1"/>
       <c r="AZ144" s="1"/>
       <c r="BA144" s="1" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="BB144" s="1"/>
       <c r="BC144" s="1"/>
       <c r="BD144" s="1"/>
       <c r="BE144" s="1"/>
-      <c r="BF144" s="1"/>
-      <c r="BG144" s="1"/>
-      <c r="BH144" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BI144" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BJ144" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="BK144" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="BL144" s="1"/>
+      <c r="BF144" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG144" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="BH144" s="1"/>
+      <c r="BI144" s="1"/>
+      <c r="BJ144" s="1"/>
+      <c r="BK144" s="1"/>
+      <c r="BL144" s="1" t="s">
+        <v>441</v>
+      </c>
       <c r="BM144" s="1"/>
       <c r="BN144" s="1"/>
-      <c r="BO144" s="1"/>
+      <c r="BO144" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="BP144" s="1"/>
       <c r="BQ144" s="1"/>
       <c r="BR144" s="1"/>
@@ -17249,21 +17245,21 @@
       <c r="CE144" s="1"/>
       <c r="CF144" s="1"/>
       <c r="CG144" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="145" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>339</v>
+        <v>135</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C145" s="26" t="s">
-        <v>382</v>
-      </c>
-      <c r="D145" s="26" t="s">
-        <v>364</v>
+      <c r="C145" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -17339,16 +17335,16 @@
       <c r="BF145" s="1"/>
       <c r="BG145" s="1"/>
       <c r="BH145" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="BI145" s="17" t="s">
-        <v>341</v>
-      </c>
-      <c r="BJ145" t="s">
-        <v>343</v>
+        <v>136</v>
+      </c>
+      <c r="BI145" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ145" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="BK145" s="1" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="BL145" s="1"/>
       <c r="BM145" s="1"/>
@@ -17362,18 +17358,10 @@
       <c r="BU145" s="1"/>
       <c r="BV145" s="1"/>
       <c r="BW145" s="1"/>
-      <c r="BX145" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="BY145" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="BZ145" t="s">
-        <v>345</v>
-      </c>
-      <c r="CA145" s="1" t="s">
-        <v>346</v>
-      </c>
+      <c r="BX145" s="1"/>
+      <c r="BY145" s="1"/>
+      <c r="BZ145" s="1"/>
+      <c r="CA145" s="1"/>
       <c r="CB145" s="1"/>
       <c r="CC145" s="1"/>
       <c r="CD145" s="1"/>
@@ -17385,16 +17373,16 @@
     </row>
     <row r="146" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>137</v>
+        <v>339</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>3</v>
+      <c r="C146" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="D146" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
@@ -17461,25 +17449,26 @@
       <c r="AY146" s="1"/>
       <c r="AZ146" s="1"/>
       <c r="BA146" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="BB146" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BD146" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BE146" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF146" s="2" t="s">
-        <v>139</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="BB146" s="1"/>
+      <c r="BC146" s="1"/>
+      <c r="BD146" s="1"/>
+      <c r="BE146" s="1"/>
+      <c r="BF146" s="1"/>
       <c r="BG146" s="1"/>
-      <c r="BH146" s="1"/>
-      <c r="BI146" s="1"/>
-      <c r="BJ146" s="1"/>
-      <c r="BK146" s="1"/>
+      <c r="BH146" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI146" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="BJ146" t="s">
+        <v>343</v>
+      </c>
+      <c r="BK146" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="BL146" s="1"/>
       <c r="BM146" s="1"/>
       <c r="BN146" s="1"/>
@@ -17492,10 +17481,18 @@
       <c r="BU146" s="1"/>
       <c r="BV146" s="1"/>
       <c r="BW146" s="1"/>
-      <c r="BX146" s="1"/>
-      <c r="BY146" s="1"/>
-      <c r="BZ146" s="1"/>
-      <c r="CA146" s="1"/>
+      <c r="BX146" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BY146" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="BZ146" t="s">
+        <v>345</v>
+      </c>
+      <c r="CA146" s="1" t="s">
+        <v>346</v>
+      </c>
       <c r="CB146" s="1"/>
       <c r="CC146" s="1"/>
       <c r="CD146" s="1"/>
@@ -17507,7 +17504,7 @@
     </row>
     <row r="147" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>367</v>
@@ -17583,18 +17580,21 @@
       <c r="AY147" s="1"/>
       <c r="AZ147" s="1"/>
       <c r="BA147" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BB147" s="1"/>
-      <c r="BC147" s="1"/>
-      <c r="BD147" s="1"/>
-      <c r="BE147" s="1"/>
-      <c r="BF147" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="BG147" s="4" t="s">
-        <v>133</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="BB147" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD147" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE147" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF147" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="BG147" s="1"/>
       <c r="BH147" s="1"/>
       <c r="BI147" s="1"/>
       <c r="BJ147" s="1"/>
@@ -17626,7 +17626,7 @@
     </row>
     <row r="148" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>367</v>
@@ -17701,25 +17701,23 @@
       <c r="AX148" s="1"/>
       <c r="AY148" s="1"/>
       <c r="AZ148" s="1"/>
-      <c r="BA148" s="1"/>
+      <c r="BA148" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="BB148" s="1"/>
       <c r="BC148" s="1"/>
       <c r="BD148" s="1"/>
       <c r="BE148" s="1"/>
-      <c r="BF148" s="1"/>
-      <c r="BG148" s="1"/>
-      <c r="BH148" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="BI148" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BJ148" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="BK148" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="BF148" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG148" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="BH148" s="1"/>
+      <c r="BI148" s="1"/>
+      <c r="BJ148" s="1"/>
+      <c r="BK148" s="1"/>
       <c r="BL148" s="1"/>
       <c r="BM148" s="1"/>
       <c r="BN148" s="1"/>
@@ -17747,15 +17745,17 @@
     </row>
     <row r="149" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D149" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
       <c r="G149" s="2" t="s">
@@ -17820,26 +17820,25 @@
       <c r="AX149" s="1"/>
       <c r="AY149" s="1"/>
       <c r="AZ149" s="1"/>
-      <c r="BA149" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="BB149" s="4" t="s">
+      <c r="BA149" s="1"/>
+      <c r="BB149" s="1"/>
+      <c r="BC149" s="1"/>
+      <c r="BD149" s="1"/>
+      <c r="BE149" s="1"/>
+      <c r="BF149" s="1"/>
+      <c r="BG149" s="1"/>
+      <c r="BH149" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI149" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="BD149" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BE149" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF149" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="BG149" s="1"/>
-      <c r="BH149" s="1"/>
-      <c r="BI149" s="1"/>
-      <c r="BJ149" s="1"/>
-      <c r="BK149" s="1"/>
+      <c r="BJ149" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="BK149" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="BL149" s="1"/>
       <c r="BM149" s="1"/>
       <c r="BN149" s="1"/>
@@ -17867,7 +17866,7 @@
     </row>
     <row r="150" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>367</v>
@@ -17941,18 +17940,21 @@
       <c r="AY150" s="1"/>
       <c r="AZ150" s="1"/>
       <c r="BA150" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BB150" s="1"/>
-      <c r="BC150" s="1"/>
-      <c r="BD150" s="1"/>
-      <c r="BE150" s="1"/>
-      <c r="BF150" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="BG150" s="4" t="s">
-        <v>133</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="BB150" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD150" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE150" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF150" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="BG150" s="1"/>
       <c r="BH150" s="1"/>
       <c r="BI150" s="1"/>
       <c r="BJ150" s="1"/>
@@ -17984,17 +17986,15 @@
     </row>
     <row r="151" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>394</v>
+        <v>144</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C151" s="26" t="s">
-        <v>395</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C151" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D151" s="1"/>
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
       <c r="G151" s="2" t="s">
@@ -18079,9 +18079,7 @@
       <c r="BL151" s="1"/>
       <c r="BM151" s="1"/>
       <c r="BN151" s="1"/>
-      <c r="BO151" s="1" t="s">
-        <v>402</v>
-      </c>
+      <c r="BO151" s="1"/>
       <c r="BP151" s="1"/>
       <c r="BQ151" s="1"/>
       <c r="BR151" s="1"/>
@@ -18105,7 +18103,7 @@
     </row>
     <row r="152" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>367</v>
@@ -18197,9 +18195,7 @@
       <c r="BI152" s="1"/>
       <c r="BJ152" s="1"/>
       <c r="BK152" s="1"/>
-      <c r="BL152" s="1" t="s">
-        <v>441</v>
-      </c>
+      <c r="BL152" s="1"/>
       <c r="BM152" s="1"/>
       <c r="BN152" s="1"/>
       <c r="BO152" s="1" t="s">
@@ -18223,12 +18219,12 @@
       <c r="CE152" s="1"/>
       <c r="CF152" s="1"/>
       <c r="CG152" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="153" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>367</v>
@@ -18325,7 +18321,9 @@
       </c>
       <c r="BM153" s="1"/>
       <c r="BN153" s="1"/>
-      <c r="BO153" s="1"/>
+      <c r="BO153" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="BP153" s="1"/>
       <c r="BQ153" s="1"/>
       <c r="BR153" s="1"/>
@@ -18344,20 +18342,22 @@
       <c r="CE153" s="1"/>
       <c r="CF153" s="1"/>
       <c r="CG153" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="154" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C154" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D154" s="1"/>
+      <c r="C154" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
       <c r="G154" s="2" t="s">
@@ -18422,26 +18422,26 @@
       <c r="AX154" s="1"/>
       <c r="AY154" s="1"/>
       <c r="AZ154" s="1"/>
-      <c r="BA154" s="1"/>
+      <c r="BA154" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="BB154" s="1"/>
       <c r="BC154" s="1"/>
       <c r="BD154" s="1"/>
       <c r="BE154" s="1"/>
-      <c r="BF154" s="1"/>
-      <c r="BG154" s="1"/>
-      <c r="BH154" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="BI154" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BJ154" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="BK154" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="BL154" s="1"/>
+      <c r="BF154" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG154" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="BH154" s="1"/>
+      <c r="BI154" s="1"/>
+      <c r="BJ154" s="1"/>
+      <c r="BK154" s="1"/>
+      <c r="BL154" s="1" t="s">
+        <v>441</v>
+      </c>
       <c r="BM154" s="1"/>
       <c r="BN154" s="1"/>
       <c r="BO154" s="1"/>
@@ -18468,21 +18468,17 @@
     </row>
     <row r="155" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C155" s="26" t="s">
-        <v>432</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C155" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D155" s="1"/>
       <c r="E155" s="1"/>
-      <c r="F155" t="s">
-        <v>3</v>
-      </c>
+      <c r="F155" s="1"/>
       <c r="G155" s="2" t="s">
         <v>53</v>
       </c>
@@ -18496,8 +18492,8 @@
       <c r="K155" t="s">
         <v>1</v>
       </c>
-      <c r="L155" s="1">
-        <v>1234567890</v>
+      <c r="L155" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="M155" s="2" t="s">
         <v>28</v>
@@ -18506,17 +18502,15 @@
         <v>236</v>
       </c>
       <c r="O155" s="1"/>
-      <c r="P155" s="1">
-        <v>122001</v>
+      <c r="P155" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
       <c r="S155" s="1"/>
       <c r="T155" s="1"/>
       <c r="U155" s="1"/>
-      <c r="V155" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="V155" s="1"/>
       <c r="W155" s="1"/>
       <c r="X155" s="1"/>
       <c r="Y155" s="1"/>
@@ -18527,19 +18521,13 @@
       <c r="AD155" s="1"/>
       <c r="AE155" s="1"/>
       <c r="AF155" s="1"/>
-      <c r="AG155" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="AG155" s="1"/>
       <c r="AH155" s="1"/>
-      <c r="AI155" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="AI155" s="1"/>
       <c r="AJ155" s="1"/>
       <c r="AK155" s="1"/>
       <c r="AL155" s="1"/>
-      <c r="AM155" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="AM155" s="1"/>
       <c r="AN155" s="1"/>
       <c r="AO155" s="1"/>
       <c r="AP155" s="1"/>
@@ -18553,26 +18541,25 @@
       <c r="AX155" s="1"/>
       <c r="AY155" s="1"/>
       <c r="AZ155" s="1"/>
-      <c r="BA155" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB155" s="4" t="s">
+      <c r="BA155" s="1"/>
+      <c r="BB155" s="1"/>
+      <c r="BC155" s="1"/>
+      <c r="BD155" s="1"/>
+      <c r="BE155" s="1"/>
+      <c r="BF155" s="1"/>
+      <c r="BG155" s="1"/>
+      <c r="BH155" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI155" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="BD155" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BE155" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF155" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="BG155" s="1"/>
-      <c r="BH155" s="1"/>
-      <c r="BI155" s="1"/>
-      <c r="BJ155" s="1"/>
-      <c r="BK155" s="1"/>
+      <c r="BJ155" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="BK155" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="BL155" s="1"/>
       <c r="BM155" s="1"/>
       <c r="BN155" s="1"/>
@@ -18600,13 +18587,13 @@
     </row>
     <row r="156" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C156" s="26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>3</v>
@@ -18628,8 +18615,8 @@
       <c r="K156" t="s">
         <v>1</v>
       </c>
-      <c r="L156" s="1" t="s">
-        <v>5</v>
+      <c r="L156" s="1">
+        <v>1234567890</v>
       </c>
       <c r="M156" s="2" t="s">
         <v>28</v>
@@ -18638,8 +18625,8 @@
         <v>236</v>
       </c>
       <c r="O156" s="1"/>
-      <c r="P156" s="1" t="s">
-        <v>124</v>
+      <c r="P156" s="1">
+        <v>122001</v>
       </c>
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
@@ -18686,18 +18673,21 @@
       <c r="AY156" s="1"/>
       <c r="AZ156" s="1"/>
       <c r="BA156" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BB156" s="1"/>
-      <c r="BC156" s="1"/>
-      <c r="BD156" s="1"/>
-      <c r="BE156" s="1"/>
-      <c r="BF156" t="s">
-        <v>149</v>
-      </c>
-      <c r="BG156" s="4" t="s">
-        <v>148</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="BB156" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD156" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE156" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF156" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="BG156" s="1"/>
       <c r="BH156" s="1"/>
       <c r="BI156" s="1"/>
       <c r="BJ156" s="1"/>
@@ -18729,13 +18719,13 @@
     </row>
     <row r="157" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C157" s="26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>3</v>
@@ -18814,25 +18804,23 @@
       <c r="AX157" s="1"/>
       <c r="AY157" s="1"/>
       <c r="AZ157" s="1"/>
-      <c r="BA157" s="1"/>
+      <c r="BA157" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="BB157" s="1"/>
       <c r="BC157" s="1"/>
       <c r="BD157" s="1"/>
       <c r="BE157" s="1"/>
-      <c r="BF157" s="1"/>
-      <c r="BG157" s="1"/>
-      <c r="BH157" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BI157" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BJ157" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="BK157" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="BF157" t="s">
+        <v>149</v>
+      </c>
+      <c r="BG157" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="BH157" s="1"/>
+      <c r="BI157" s="1"/>
+      <c r="BJ157" s="1"/>
+      <c r="BK157" s="1"/>
       <c r="BL157" s="1"/>
       <c r="BM157" s="1"/>
       <c r="BN157" s="1"/>
@@ -18860,13 +18848,13 @@
     </row>
     <row r="158" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>314</v>
+        <v>150</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C158" s="26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>3</v>
@@ -18946,15 +18934,24 @@
       <c r="AY158" s="1"/>
       <c r="AZ158" s="1"/>
       <c r="BA158" s="1"/>
-      <c r="BB158" s="4"/>
-      <c r="BD158" s="2"/>
-      <c r="BE158" s="3"/>
-      <c r="BF158" s="2"/>
+      <c r="BB158" s="1"/>
+      <c r="BC158" s="1"/>
+      <c r="BD158" s="1"/>
+      <c r="BE158" s="1"/>
+      <c r="BF158" s="1"/>
       <c r="BG158" s="1"/>
-      <c r="BH158" s="1"/>
-      <c r="BI158" s="1"/>
-      <c r="BJ158" s="1"/>
-      <c r="BK158" s="1"/>
+      <c r="BH158" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="BI158" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ158" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="BK158" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="BL158" s="1"/>
       <c r="BM158" s="1"/>
       <c r="BN158" s="1"/>
@@ -18981,32 +18978,56 @@
       </c>
     </row>
     <row r="159" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A159" s="9" t="s">
-        <v>242</v>
+      <c r="A159" s="2" t="s">
+        <v>314</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
+      <c r="C159" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E159" s="1"/>
-      <c r="F159" s="1"/>
-      <c r="G159" s="1"/>
-      <c r="H159" s="1"/>
+      <c r="F159" t="s">
+        <v>3</v>
+      </c>
+      <c r="G159" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H159" s="3" t="s">
+        <v>327</v>
+      </c>
       <c r="I159" s="1"/>
-      <c r="J159" s="1"/>
-      <c r="K159" s="1"/>
-      <c r="L159" s="1"/>
-      <c r="M159" s="1"/>
-      <c r="N159" s="1"/>
+      <c r="J159" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K159" t="s">
+        <v>1</v>
+      </c>
+      <c r="L159" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M159" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N159" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="O159" s="1"/>
-      <c r="P159" s="1"/>
+      <c r="P159" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
       <c r="S159" s="1"/>
       <c r="T159" s="1"/>
       <c r="U159" s="1"/>
-      <c r="V159" s="1"/>
+      <c r="V159" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="W159" s="1"/>
       <c r="X159" s="1"/>
       <c r="Y159" s="1"/>
@@ -19017,13 +19038,19 @@
       <c r="AD159" s="1"/>
       <c r="AE159" s="1"/>
       <c r="AF159" s="1"/>
-      <c r="AG159" s="1"/>
+      <c r="AG159" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AH159" s="1"/>
-      <c r="AI159" s="1"/>
+      <c r="AI159" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AJ159" s="1"/>
       <c r="AK159" s="1"/>
       <c r="AL159" s="1"/>
-      <c r="AM159" s="1"/>
+      <c r="AM159" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AN159" s="1"/>
       <c r="AO159" s="1"/>
       <c r="AP159" s="1"/>
@@ -19038,14 +19065,13 @@
       <c r="AY159" s="1"/>
       <c r="AZ159" s="1"/>
       <c r="BA159" s="1"/>
-      <c r="BB159" s="1"/>
-      <c r="BC159" s="1"/>
-      <c r="BD159" s="1"/>
-      <c r="BE159" s="1"/>
-      <c r="BF159" s="1"/>
+      <c r="BB159" s="4"/>
+      <c r="BD159" s="2"/>
+      <c r="BE159" s="3"/>
+      <c r="BF159" s="2"/>
       <c r="BG159" s="1"/>
       <c r="BH159" s="1"/>
-      <c r="BI159" s="11"/>
+      <c r="BI159" s="1"/>
       <c r="BJ159" s="1"/>
       <c r="BK159" s="1"/>
       <c r="BL159" s="1"/>
@@ -19069,66 +19095,36 @@
       <c r="CD159" s="1"/>
       <c r="CE159" s="1"/>
       <c r="CF159" s="1"/>
-      <c r="CG159" s="1"/>
+      <c r="CG159" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="160" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
-        <v>250</v>
+      <c r="A160" s="9" t="s">
+        <v>242</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C160" s="28" t="s">
-        <v>387</v>
-      </c>
-      <c r="D160" s="11" t="s">
-        <v>364</v>
-      </c>
-      <c r="E160" s="3"/>
-      <c r="F160" s="3"/>
-      <c r="G160" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H160" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="I160" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="J160" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="K160" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="L160" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="M160" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N160" s="1" t="s">
-        <v>236</v>
-      </c>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
       <c r="O160" s="1"/>
-      <c r="P160" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q160" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="R160" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="S160" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="T160" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="U160" s="1" t="s">
-        <v>248</v>
-      </c>
+      <c r="P160" s="1"/>
+      <c r="Q160" s="1"/>
+      <c r="R160" s="1"/>
+      <c r="S160" s="1"/>
+      <c r="T160" s="1"/>
+      <c r="U160" s="1"/>
       <c r="V160" s="1"/>
       <c r="W160" s="1"/>
       <c r="X160" s="1"/>
@@ -19140,9 +19136,7 @@
       <c r="AD160" s="1"/>
       <c r="AE160" s="1"/>
       <c r="AF160" s="1"/>
-      <c r="AG160" s="1" t="s">
-        <v>353</v>
-      </c>
+      <c r="AG160" s="1"/>
       <c r="AH160" s="1"/>
       <c r="AI160" s="1"/>
       <c r="AJ160" s="1"/>
@@ -19162,21 +19156,12 @@
       <c r="AX160" s="1"/>
       <c r="AY160" s="1"/>
       <c r="AZ160" s="1"/>
-      <c r="BA160" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB160" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BD160" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BE160" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF160" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="BA160" s="1"/>
+      <c r="BB160" s="1"/>
+      <c r="BC160" s="1"/>
+      <c r="BD160" s="1"/>
+      <c r="BE160" s="1"/>
+      <c r="BF160" s="1"/>
       <c r="BG160" s="1"/>
       <c r="BH160" s="1"/>
       <c r="BI160" s="11"/>
@@ -19202,14 +19187,12 @@
       <c r="CC160" s="1"/>
       <c r="CD160" s="1"/>
       <c r="CE160" s="1"/>
-      <c r="CF160" s="18"/>
-      <c r="CG160" t="s">
-        <v>368</v>
-      </c>
+      <c r="CF160" s="1"/>
+      <c r="CG160" s="1"/>
     </row>
     <row r="161" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>367</v>
@@ -19223,22 +19206,22 @@
       <c r="E161" s="3"/>
       <c r="F161" s="3"/>
       <c r="G161" s="3" t="s">
-        <v>6</v>
+        <v>243</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>6</v>
+        <v>244</v>
       </c>
       <c r="I161" s="1" t="s">
         <v>436</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>384</v>
+        <v>317</v>
       </c>
       <c r="K161" s="2" t="s">
-        <v>385</v>
+        <v>351</v>
       </c>
       <c r="L161" s="1" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="M161" s="2" t="s">
         <v>28</v>
@@ -19277,7 +19260,7 @@
       <c r="AE161" s="1"/>
       <c r="AF161" s="1"/>
       <c r="AG161" s="1" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
       <c r="AH161" s="1"/>
       <c r="AI161" s="1"/>
@@ -19340,12 +19323,12 @@
       <c r="CE161" s="1"/>
       <c r="CF161" s="18"/>
       <c r="CG161" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="162" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>367</v>
@@ -19358,19 +19341,23 @@
       </c>
       <c r="E162" s="3"/>
       <c r="F162" s="3"/>
-      <c r="G162" s="3"/>
-      <c r="H162" s="1"/>
+      <c r="G162" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="I162" s="1" t="s">
         <v>436</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>317</v>
+        <v>384</v>
       </c>
       <c r="K162" s="2" t="s">
-        <v>351</v>
+        <v>385</v>
       </c>
       <c r="L162" s="1" t="s">
-        <v>318</v>
+        <v>365</v>
       </c>
       <c r="M162" s="2" t="s">
         <v>28</v>
@@ -19409,7 +19396,7 @@
       <c r="AE162" s="1"/>
       <c r="AF162" s="1"/>
       <c r="AG162" s="1" t="s">
-        <v>353</v>
+        <v>386</v>
       </c>
       <c r="AH162" s="1"/>
       <c r="AI162" s="1"/>
@@ -19430,12 +19417,21 @@
       <c r="AX162" s="1"/>
       <c r="AY162" s="1"/>
       <c r="AZ162" s="1"/>
-      <c r="BA162" s="1"/>
-      <c r="BB162" s="1"/>
-      <c r="BC162" s="12"/>
-      <c r="BD162" s="1"/>
-      <c r="BE162" s="1"/>
-      <c r="BF162" s="1"/>
+      <c r="BA162" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BB162" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD162" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE162" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF162" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="BG162" s="1"/>
       <c r="BH162" s="1"/>
       <c r="BI162" s="11"/>
@@ -19463,49 +19459,43 @@
       <c r="CE162" s="1"/>
       <c r="CF162" s="18"/>
       <c r="CG162" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="163" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C163" s="28" t="s">
-        <v>437</v>
+        <v>387</v>
       </c>
       <c r="D163" s="11" t="s">
         <v>364</v>
       </c>
       <c r="E163" s="3"/>
-      <c r="F163" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="G163" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H163" s="1" t="s">
-        <v>244</v>
-      </c>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3"/>
+      <c r="H163" s="1"/>
       <c r="I163" s="1" t="s">
         <v>436</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>376</v>
+        <v>317</v>
       </c>
       <c r="K163" s="2" t="s">
-        <v>377</v>
+        <v>351</v>
       </c>
       <c r="L163" s="1" t="s">
-        <v>375</v>
+        <v>318</v>
       </c>
       <c r="M163" s="2" t="s">
-        <v>372</v>
+        <v>28</v>
       </c>
       <c r="N163" s="1" t="s">
-        <v>373</v>
+        <v>236</v>
       </c>
       <c r="O163" s="1"/>
       <c r="P163" s="1" t="s">
@@ -19538,7 +19528,7 @@
       <c r="AE163" s="1"/>
       <c r="AF163" s="1"/>
       <c r="AG163" s="1" t="s">
-        <v>374</v>
+        <v>353</v>
       </c>
       <c r="AH163" s="1"/>
       <c r="AI163" s="1"/>
@@ -19596,20 +19586,22 @@
       </c>
     </row>
     <row r="164" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A164" s="7" t="s">
-        <v>254</v>
+      <c r="A164" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C164" s="28" t="s">
-        <v>387</v>
+        <v>437</v>
       </c>
       <c r="D164" s="11" t="s">
         <v>364</v>
       </c>
       <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
+      <c r="F164" s="3" t="s">
+        <v>364</v>
+      </c>
       <c r="G164" s="3" t="s">
         <v>243</v>
       </c>
@@ -19620,19 +19612,19 @@
         <v>436</v>
       </c>
       <c r="J164" s="1" t="s">
-        <v>317</v>
+        <v>376</v>
       </c>
       <c r="K164" s="2" t="s">
-        <v>351</v>
+        <v>377</v>
       </c>
       <c r="L164" s="1" t="s">
-        <v>318</v>
+        <v>375</v>
       </c>
       <c r="M164" s="2" t="s">
-        <v>28</v>
+        <v>372</v>
       </c>
       <c r="N164" s="1" t="s">
-        <v>236</v>
+        <v>373</v>
       </c>
       <c r="O164" s="1"/>
       <c r="P164" s="1" t="s">
@@ -19665,7 +19657,7 @@
       <c r="AE164" s="1"/>
       <c r="AF164" s="1"/>
       <c r="AG164" s="1" t="s">
-        <v>353</v>
+        <v>374</v>
       </c>
       <c r="AH164" s="1"/>
       <c r="AI164" s="1"/>
@@ -19686,21 +19678,12 @@
       <c r="AX164" s="1"/>
       <c r="AY164" s="1"/>
       <c r="AZ164" s="1"/>
-      <c r="BA164" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB164" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BD164" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BE164" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF164" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="BA164" s="1"/>
+      <c r="BB164" s="1"/>
+      <c r="BC164" s="12"/>
+      <c r="BD164" s="1"/>
+      <c r="BE164" s="1"/>
+      <c r="BF164" s="1"/>
       <c r="BG164" s="1"/>
       <c r="BH164" s="1"/>
       <c r="BI164" s="11"/>
@@ -19733,7 +19716,7 @@
     </row>
     <row r="165" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>367</v>
@@ -19746,8 +19729,12 @@
       </c>
       <c r="E165" s="3"/>
       <c r="F165" s="3"/>
-      <c r="G165" s="3"/>
-      <c r="H165" s="1"/>
+      <c r="G165" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>244</v>
+      </c>
       <c r="I165" s="1" t="s">
         <v>436</v>
       </c>
@@ -19865,7 +19852,7 @@
     </row>
     <row r="166" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>367</v>
@@ -19997,38 +19984,32 @@
     </row>
     <row r="167" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C167" s="28" t="s">
-        <v>438</v>
+        <v>387</v>
       </c>
       <c r="D167" s="11" t="s">
         <v>364</v>
       </c>
       <c r="E167" s="3"/>
-      <c r="F167" s="11" t="s">
-        <v>364</v>
-      </c>
-      <c r="G167" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H167" s="1" t="s">
-        <v>244</v>
-      </c>
+      <c r="F167" s="3"/>
+      <c r="G167" s="3"/>
+      <c r="H167" s="1"/>
       <c r="I167" s="1" t="s">
         <v>436</v>
       </c>
       <c r="J167" s="1" t="s">
-        <v>388</v>
+        <v>317</v>
       </c>
       <c r="K167" s="2" t="s">
-        <v>389</v>
+        <v>351</v>
       </c>
       <c r="L167" s="1" t="s">
-        <v>246</v>
+        <v>318</v>
       </c>
       <c r="M167" s="2" t="s">
         <v>28</v>
@@ -20067,7 +20048,7 @@
       <c r="AE167" s="1"/>
       <c r="AF167" s="1"/>
       <c r="AG167" s="1" t="s">
-        <v>390</v>
+        <v>353</v>
       </c>
       <c r="AH167" s="1"/>
       <c r="AI167" s="1"/>
@@ -20119,14 +20100,14 @@
       <c r="BT167" s="1"/>
       <c r="BU167" s="1"/>
       <c r="BV167" s="1"/>
-      <c r="BW167" s="12"/>
-      <c r="BX167" s="12"/>
-      <c r="BY167" s="12"/>
-      <c r="BZ167" s="12"/>
-      <c r="CA167" s="12"/>
-      <c r="CB167" s="12"/>
-      <c r="CC167" s="12"/>
-      <c r="CD167" s="12"/>
+      <c r="BW167" s="1"/>
+      <c r="BX167" s="1"/>
+      <c r="BY167" s="1"/>
+      <c r="BZ167" s="1"/>
+      <c r="CA167" s="1"/>
+      <c r="CB167" s="1"/>
+      <c r="CC167" s="1"/>
+      <c r="CD167" s="1"/>
       <c r="CE167" s="1"/>
       <c r="CF167" s="18"/>
       <c r="CG167" t="s">
@@ -20135,40 +20116,64 @@
     </row>
     <row r="168" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>286</v>
+        <v>257</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C168" s="11" t="s">
-        <v>2</v>
+      <c r="C168" s="28" t="s">
+        <v>438</v>
       </c>
       <c r="D168" s="11" t="s">
-        <v>3</v>
+        <v>364</v>
       </c>
       <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
+      <c r="F168" s="11" t="s">
+        <v>364</v>
+      </c>
       <c r="G168" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H168" s="3" t="s">
-        <v>59</v>
+        <v>243</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="I168" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="J168" s="1"/>
-      <c r="K168" s="2"/>
-      <c r="L168" s="1"/>
-      <c r="M168" s="2"/>
-      <c r="N168" s="1"/>
+      <c r="J168" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="K168" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="L168" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="M168" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N168" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="O168" s="1"/>
-      <c r="P168" s="1"/>
-      <c r="Q168" s="11"/>
-      <c r="R168" s="10"/>
-      <c r="S168" s="10"/>
-      <c r="T168" s="1"/>
-      <c r="U168" s="1"/>
+      <c r="P168" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q168" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="R168" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="S168" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="T168" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="U168" s="1" t="s">
+        <v>248</v>
+      </c>
       <c r="V168" s="1"/>
       <c r="W168" s="1"/>
       <c r="X168" s="1"/>
@@ -20180,7 +20185,9 @@
       <c r="AD168" s="1"/>
       <c r="AE168" s="1"/>
       <c r="AF168" s="1"/>
-      <c r="AG168" s="1"/>
+      <c r="AG168" s="1" t="s">
+        <v>390</v>
+      </c>
       <c r="AH168" s="1"/>
       <c r="AI168" s="1"/>
       <c r="AJ168" s="1"/>
@@ -20200,18 +20207,24 @@
       <c r="AX168" s="1"/>
       <c r="AY168" s="1"/>
       <c r="AZ168" s="1"/>
-      <c r="BA168" s="1"/>
-      <c r="BB168" s="4"/>
-      <c r="BD168" s="2"/>
-      <c r="BE168" s="3"/>
-      <c r="BF168" s="2"/>
+      <c r="BA168" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BB168" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD168" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE168" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF168" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="BG168" s="1"/>
-      <c r="BH168" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="BI168" s="11" t="s">
-        <v>354</v>
-      </c>
+      <c r="BH168" s="1"/>
+      <c r="BI168" s="11"/>
       <c r="BJ168" s="1"/>
       <c r="BK168" s="1"/>
       <c r="BL168" s="1"/>
@@ -20236,21 +20249,21 @@
       <c r="CE168" s="1"/>
       <c r="CF168" s="18"/>
       <c r="CG168" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="169" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C169" s="28" t="s">
-        <v>287</v>
-      </c>
-      <c r="D169" s="28" t="s">
-        <v>391</v>
+      <c r="C169" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D169" s="11" t="s">
+        <v>3</v>
       </c>
       <c r="E169" s="3"/>
       <c r="F169" s="3"/>
@@ -20263,28 +20276,16 @@
       <c r="I169" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="J169" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K169" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L169" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M169" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N169" s="1" t="s">
-        <v>236</v>
-      </c>
+      <c r="J169" s="1"/>
+      <c r="K169" s="2"/>
+      <c r="L169" s="1"/>
+      <c r="M169" s="2"/>
+      <c r="N169" s="1"/>
       <c r="O169" s="1"/>
-      <c r="P169" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="P169" s="1"/>
       <c r="Q169" s="11"/>
-      <c r="R169" s="1"/>
-      <c r="S169" s="1"/>
+      <c r="R169" s="10"/>
+      <c r="S169" s="10"/>
       <c r="T169" s="1"/>
       <c r="U169" s="1"/>
       <c r="V169" s="1"/>
@@ -20318,9 +20319,7 @@
       <c r="AX169" s="1"/>
       <c r="AY169" s="1"/>
       <c r="AZ169" s="1"/>
-      <c r="BA169" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="BA169" s="1"/>
       <c r="BB169" s="4"/>
       <c r="BD169" s="2"/>
       <c r="BE169" s="3"/>
@@ -20330,14 +20329,10 @@
         <v>288</v>
       </c>
       <c r="BI169" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="BJ169" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="BK169" s="1" t="s">
-        <v>355</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="BJ169" s="1"/>
+      <c r="BK169" s="1"/>
       <c r="BL169" s="1"/>
       <c r="BM169" s="1"/>
       <c r="BN169" s="1"/>
@@ -20363,9 +20358,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="170" spans="1:85" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>367</v>
@@ -20378,39 +20373,39 @@
       </c>
       <c r="E170" s="3"/>
       <c r="F170" s="3"/>
-      <c r="G170" s="3"/>
-      <c r="H170" s="3"/>
+      <c r="G170" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="I170" s="1" t="s">
         <v>436</v>
       </c>
       <c r="J170" s="2" t="s">
-        <v>294</v>
+        <v>0</v>
       </c>
       <c r="K170" s="2" t="s">
-        <v>295</v>
+        <v>1</v>
       </c>
       <c r="L170" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="M170" s="2"/>
-      <c r="N170" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="M170" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N170" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="O170" s="1"/>
-      <c r="P170" s="1"/>
-      <c r="Q170" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="R170" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="S170" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="T170" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="U170" s="1" t="s">
-        <v>298</v>
-      </c>
+      <c r="P170" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q170" s="11"/>
+      <c r="R170" s="1"/>
+      <c r="S170" s="1"/>
+      <c r="T170" s="1"/>
+      <c r="U170" s="1"/>
       <c r="V170" s="1"/>
       <c r="W170" s="1"/>
       <c r="X170" s="1"/>
@@ -20422,9 +20417,7 @@
       <c r="AD170" s="1"/>
       <c r="AE170" s="1"/>
       <c r="AF170" s="1"/>
-      <c r="AG170" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="AG170" s="1"/>
       <c r="AH170" s="1"/>
       <c r="AI170" s="1"/>
       <c r="AJ170" s="1"/>
@@ -20444,20 +20437,28 @@
       <c r="AX170" s="1"/>
       <c r="AY170" s="1"/>
       <c r="AZ170" s="1"/>
-      <c r="BA170" s="1"/>
+      <c r="BA170" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="BB170" s="4"/>
       <c r="BD170" s="2"/>
       <c r="BE170" s="3"/>
       <c r="BF170" s="2"/>
       <c r="BG170" s="1"/>
-      <c r="BH170" s="1"/>
-      <c r="BI170" s="11"/>
-      <c r="BJ170" s="1"/>
-      <c r="BK170" s="1"/>
+      <c r="BH170" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="BI170" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="BJ170" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="BK170" s="1" t="s">
+        <v>355</v>
+      </c>
       <c r="BL170" s="1"/>
-      <c r="BM170" s="1" t="s">
-        <v>296</v>
-      </c>
+      <c r="BM170" s="1"/>
       <c r="BN170" s="1"/>
       <c r="BO170" s="1"/>
       <c r="BP170" s="1"/>
@@ -20481,50 +20482,54 @@
         <v>366</v>
       </c>
     </row>
-    <row r="171" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>442</v>
+    <row r="171" spans="1:85" ht="30" x14ac:dyDescent="0.25">
+      <c r="A171" s="7" t="s">
+        <v>290</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C171" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D171" s="1"/>
-      <c r="E171" s="1"/>
-      <c r="F171" s="1"/>
-      <c r="G171" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H171" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="I171" s="1"/>
+      <c r="C171" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="D171" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="E171" s="3"/>
+      <c r="F171" s="3"/>
+      <c r="G171" s="3"/>
+      <c r="H171" s="3"/>
+      <c r="I171" s="1" t="s">
+        <v>436</v>
+      </c>
       <c r="J171" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K171" t="s">
-        <v>1</v>
+        <v>294</v>
+      </c>
+      <c r="K171" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="L171" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M171" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N171" s="1" t="s">
-        <v>236</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="M171" s="2"/>
+      <c r="N171" s="1"/>
       <c r="O171" s="1"/>
-      <c r="P171" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q171" s="1"/>
-      <c r="R171" s="1"/>
-      <c r="S171" s="1"/>
-      <c r="T171" s="1"/>
-      <c r="U171" s="1"/>
+      <c r="P171" s="1"/>
+      <c r="Q171" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="R171" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="S171" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="T171" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="U171" s="1" t="s">
+        <v>298</v>
+      </c>
       <c r="V171" s="1"/>
       <c r="W171" s="1"/>
       <c r="X171" s="1"/>
@@ -20536,7 +20541,9 @@
       <c r="AD171" s="1"/>
       <c r="AE171" s="1"/>
       <c r="AF171" s="1"/>
-      <c r="AG171" s="1"/>
+      <c r="AG171" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="AH171" s="1"/>
       <c r="AI171" s="1"/>
       <c r="AJ171" s="1"/>
@@ -20556,25 +20563,20 @@
       <c r="AX171" s="1"/>
       <c r="AY171" s="1"/>
       <c r="AZ171" s="1"/>
-      <c r="BA171" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BB171" s="1"/>
-      <c r="BC171" s="1"/>
-      <c r="BD171" s="1"/>
-      <c r="BE171" s="1"/>
-      <c r="BF171" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="BG171" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="BA171" s="1"/>
+      <c r="BB171" s="4"/>
+      <c r="BD171" s="2"/>
+      <c r="BE171" s="3"/>
+      <c r="BF171" s="2"/>
+      <c r="BG171" s="1"/>
       <c r="BH171" s="1"/>
-      <c r="BI171" s="1"/>
+      <c r="BI171" s="11"/>
       <c r="BJ171" s="1"/>
       <c r="BK171" s="1"/>
       <c r="BL171" s="1"/>
-      <c r="BM171" s="1"/>
+      <c r="BM171" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="BN171" s="1"/>
       <c r="BO171" s="1"/>
       <c r="BP171" s="1"/>
@@ -20584,45 +20586,59 @@
       <c r="BT171" s="1"/>
       <c r="BU171" s="1"/>
       <c r="BV171" s="1"/>
-      <c r="BW171" s="1"/>
-      <c r="BX171" s="1"/>
-      <c r="BY171" s="1"/>
-      <c r="BZ171" s="1"/>
-      <c r="CA171" s="1"/>
-      <c r="CB171" s="1"/>
-      <c r="CC171" s="1"/>
-      <c r="CD171" s="1"/>
+      <c r="BW171" s="12"/>
+      <c r="BX171" s="12"/>
+      <c r="BY171" s="12"/>
+      <c r="BZ171" s="12"/>
+      <c r="CA171" s="12"/>
+      <c r="CB171" s="12"/>
+      <c r="CC171" s="12"/>
+      <c r="CD171" s="12"/>
       <c r="CE171" s="1"/>
-      <c r="CF171" s="1"/>
+      <c r="CF171" s="18"/>
       <c r="CG171" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="172" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A172" s="7" t="s">
-        <v>443</v>
+      <c r="A172" s="2" t="s">
+        <v>442</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C172" s="11"/>
+      <c r="C172" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
       <c r="F172" s="1"/>
-      <c r="G172" s="1" t="s">
+      <c r="G172" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H172" s="1" t="s">
-        <v>444</v>
+      <c r="H172" s="3" t="s">
+        <v>327</v>
       </c>
       <c r="I172" s="1"/>
-      <c r="J172" s="1"/>
-      <c r="K172" s="1"/>
-      <c r="L172" s="1"/>
-      <c r="M172" s="1"/>
-      <c r="N172" s="1"/>
+      <c r="J172" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K172" t="s">
+        <v>1</v>
+      </c>
+      <c r="L172" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M172" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N172" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="O172" s="1"/>
-      <c r="P172" s="1"/>
+      <c r="P172" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
       <c r="S172" s="1"/>
@@ -20659,15 +20675,21 @@
       <c r="AX172" s="1"/>
       <c r="AY172" s="1"/>
       <c r="AZ172" s="1"/>
-      <c r="BA172" s="1"/>
+      <c r="BA172" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="BB172" s="1"/>
       <c r="BC172" s="1"/>
       <c r="BD172" s="1"/>
       <c r="BE172" s="1"/>
-      <c r="BF172" s="1"/>
-      <c r="BG172" s="1"/>
+      <c r="BF172" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG172" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="BH172" s="1"/>
-      <c r="BI172" s="11"/>
+      <c r="BI172" s="1"/>
       <c r="BJ172" s="1"/>
       <c r="BK172" s="1"/>
       <c r="BL172" s="1"/>
@@ -20690,50 +20712,36 @@
       <c r="CC172" s="1"/>
       <c r="CD172" s="1"/>
       <c r="CE172" s="1"/>
-      <c r="CF172" s="18"/>
+      <c r="CF172" s="1"/>
       <c r="CG172" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="173" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
-        <v>445</v>
+      <c r="A173" s="7" t="s">
+        <v>443</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C173" s="1" t="s">
-        <v>331</v>
-      </c>
+      <c r="C173" s="11"/>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
-      <c r="G173" s="2" t="s">
+      <c r="G173" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H173" s="3" t="s">
+      <c r="H173" s="1" t="s">
         <v>444</v>
       </c>
       <c r="I173" s="1"/>
-      <c r="J173" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K173" t="s">
-        <v>1</v>
-      </c>
-      <c r="L173" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M173" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N173" s="1" t="s">
-        <v>236</v>
-      </c>
+      <c r="J173" s="1"/>
+      <c r="K173" s="1"/>
+      <c r="L173" s="1"/>
+      <c r="M173" s="1"/>
+      <c r="N173" s="1"/>
       <c r="O173" s="1"/>
-      <c r="P173" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="P173" s="1"/>
       <c r="Q173" s="1"/>
       <c r="R173" s="1"/>
       <c r="S173" s="1"/>
@@ -20776,9 +20784,9 @@
       <c r="BD173" s="1"/>
       <c r="BE173" s="1"/>
       <c r="BF173" s="1"/>
-      <c r="BG173" s="4"/>
+      <c r="BG173" s="1"/>
       <c r="BH173" s="1"/>
-      <c r="BI173" s="1"/>
+      <c r="BI173" s="11"/>
       <c r="BJ173" s="1"/>
       <c r="BK173" s="1"/>
       <c r="BL173" s="1"/>
@@ -20801,28 +20809,50 @@
       <c r="CC173" s="1"/>
       <c r="CD173" s="1"/>
       <c r="CE173" s="1"/>
-      <c r="CF173" s="1"/>
+      <c r="CF173" s="18"/>
       <c r="CG173" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="174" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A174" s="7"/>
-      <c r="B174" s="1"/>
-      <c r="C174" s="1"/>
+      <c r="A174" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
-      <c r="G174" s="1"/>
-      <c r="H174" s="1"/>
+      <c r="G174" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H174" s="3" t="s">
+        <v>444</v>
+      </c>
       <c r="I174" s="1"/>
-      <c r="J174" s="1"/>
-      <c r="K174" s="1"/>
-      <c r="L174" s="1"/>
-      <c r="M174" s="1"/>
-      <c r="N174" s="1"/>
+      <c r="J174" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K174" t="s">
+        <v>1</v>
+      </c>
+      <c r="L174" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M174" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N174" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="O174" s="1"/>
-      <c r="P174" s="1"/>
+      <c r="P174" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="Q174" s="1"/>
       <c r="R174" s="1"/>
       <c r="S174" s="1"/>
@@ -20865,9 +20895,9 @@
       <c r="BD174" s="1"/>
       <c r="BE174" s="1"/>
       <c r="BF174" s="1"/>
-      <c r="BG174" s="1"/>
+      <c r="BG174" s="4"/>
       <c r="BH174" s="1"/>
-      <c r="BI174" s="11"/>
+      <c r="BI174" s="1"/>
       <c r="BJ174" s="1"/>
       <c r="BK174" s="1"/>
       <c r="BL174" s="1"/>
@@ -20891,7 +20921,9 @@
       <c r="CD174" s="1"/>
       <c r="CE174" s="1"/>
       <c r="CF174" s="1"/>
-      <c r="CG174" s="1"/>
+      <c r="CG174" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="175" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A175" s="7"/>
@@ -22027,7 +22059,7 @@
     <row r="188" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A188" s="7"/>
       <c r="B188" s="1"/>
-      <c r="C188" s="11"/>
+      <c r="C188" s="1"/>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
       <c r="F188" s="1"/>
@@ -23852,91 +23884,91 @@
       <c r="CG208" s="1"/>
     </row>
     <row r="209" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A209" s="8"/>
-      <c r="B209" s="2"/>
-      <c r="C209" s="3"/>
-      <c r="D209" s="2"/>
-      <c r="E209" s="2"/>
-      <c r="F209" s="2"/>
-      <c r="G209" s="2"/>
-      <c r="H209" s="2"/>
-      <c r="I209" s="2"/>
-      <c r="J209" s="2"/>
-      <c r="K209" s="2"/>
-      <c r="L209" s="2"/>
-      <c r="M209" s="2"/>
-      <c r="N209" s="2"/>
-      <c r="O209" s="2"/>
-      <c r="P209" s="2"/>
-      <c r="Q209" s="2"/>
-      <c r="R209" s="2"/>
-      <c r="S209" s="2"/>
-      <c r="T209" s="2"/>
-      <c r="U209" s="2"/>
-      <c r="V209" s="2"/>
-      <c r="W209" s="2"/>
-      <c r="X209" s="2"/>
-      <c r="Y209" s="2"/>
-      <c r="Z209" s="2"/>
-      <c r="AA209" s="2"/>
-      <c r="AB209" s="2"/>
-      <c r="AC209" s="2"/>
-      <c r="AD209" s="2"/>
-      <c r="AE209" s="2"/>
-      <c r="AF209" s="2"/>
-      <c r="AG209" s="2"/>
-      <c r="AH209" s="2"/>
-      <c r="AI209" s="2"/>
-      <c r="AJ209" s="2"/>
-      <c r="AK209" s="2"/>
-      <c r="AL209" s="2"/>
-      <c r="AM209" s="2"/>
-      <c r="AN209" s="2"/>
-      <c r="AO209" s="2"/>
-      <c r="AP209" s="2"/>
-      <c r="AQ209" s="2"/>
-      <c r="AR209" s="2"/>
-      <c r="AS209" s="2"/>
-      <c r="AT209" s="2"/>
-      <c r="AU209" s="2"/>
-      <c r="AV209" s="2"/>
-      <c r="AW209" s="2"/>
-      <c r="AX209" s="2"/>
-      <c r="AY209" s="2"/>
-      <c r="AZ209" s="2"/>
-      <c r="BA209" s="2"/>
-      <c r="BB209" s="2"/>
-      <c r="BC209" s="2"/>
-      <c r="BD209" s="2"/>
-      <c r="BE209" s="2"/>
-      <c r="BF209" s="2"/>
-      <c r="BG209" s="2"/>
-      <c r="BH209" s="2"/>
-      <c r="BI209" s="3"/>
-      <c r="BJ209" s="2"/>
-      <c r="BK209" s="2"/>
-      <c r="BL209" s="2"/>
-      <c r="BM209" s="2"/>
-      <c r="BN209" s="2"/>
-      <c r="BO209" s="2"/>
-      <c r="BP209" s="2"/>
-      <c r="BQ209" s="2"/>
-      <c r="BR209" s="2"/>
-      <c r="BS209" s="2"/>
-      <c r="BT209" s="2"/>
-      <c r="BU209" s="2"/>
-      <c r="BV209" s="2"/>
-      <c r="BW209" s="2"/>
-      <c r="BX209" s="2"/>
-      <c r="BY209" s="2"/>
-      <c r="BZ209" s="2"/>
-      <c r="CA209" s="2"/>
-      <c r="CB209" s="2"/>
-      <c r="CC209" s="2"/>
-      <c r="CD209" s="2"/>
-      <c r="CE209" s="2"/>
-      <c r="CF209" s="2"/>
-      <c r="CG209" s="2"/>
+      <c r="A209" s="7"/>
+      <c r="B209" s="1"/>
+      <c r="C209" s="11"/>
+      <c r="D209" s="1"/>
+      <c r="E209" s="1"/>
+      <c r="F209" s="1"/>
+      <c r="G209" s="1"/>
+      <c r="H209" s="1"/>
+      <c r="I209" s="1"/>
+      <c r="J209" s="1"/>
+      <c r="K209" s="1"/>
+      <c r="L209" s="1"/>
+      <c r="M209" s="1"/>
+      <c r="N209" s="1"/>
+      <c r="O209" s="1"/>
+      <c r="P209" s="1"/>
+      <c r="Q209" s="1"/>
+      <c r="R209" s="1"/>
+      <c r="S209" s="1"/>
+      <c r="T209" s="1"/>
+      <c r="U209" s="1"/>
+      <c r="V209" s="1"/>
+      <c r="W209" s="1"/>
+      <c r="X209" s="1"/>
+      <c r="Y209" s="1"/>
+      <c r="Z209" s="1"/>
+      <c r="AA209" s="1"/>
+      <c r="AB209" s="1"/>
+      <c r="AC209" s="1"/>
+      <c r="AD209" s="1"/>
+      <c r="AE209" s="1"/>
+      <c r="AF209" s="1"/>
+      <c r="AG209" s="1"/>
+      <c r="AH209" s="1"/>
+      <c r="AI209" s="1"/>
+      <c r="AJ209" s="1"/>
+      <c r="AK209" s="1"/>
+      <c r="AL209" s="1"/>
+      <c r="AM209" s="1"/>
+      <c r="AN209" s="1"/>
+      <c r="AO209" s="1"/>
+      <c r="AP209" s="1"/>
+      <c r="AQ209" s="1"/>
+      <c r="AR209" s="1"/>
+      <c r="AS209" s="1"/>
+      <c r="AT209" s="1"/>
+      <c r="AU209" s="1"/>
+      <c r="AV209" s="1"/>
+      <c r="AW209" s="1"/>
+      <c r="AX209" s="1"/>
+      <c r="AY209" s="1"/>
+      <c r="AZ209" s="1"/>
+      <c r="BA209" s="1"/>
+      <c r="BB209" s="1"/>
+      <c r="BC209" s="1"/>
+      <c r="BD209" s="1"/>
+      <c r="BE209" s="1"/>
+      <c r="BF209" s="1"/>
+      <c r="BG209" s="1"/>
+      <c r="BH209" s="1"/>
+      <c r="BI209" s="11"/>
+      <c r="BJ209" s="1"/>
+      <c r="BK209" s="1"/>
+      <c r="BL209" s="1"/>
+      <c r="BM209" s="1"/>
+      <c r="BN209" s="1"/>
+      <c r="BO209" s="1"/>
+      <c r="BP209" s="1"/>
+      <c r="BQ209" s="1"/>
+      <c r="BR209" s="1"/>
+      <c r="BS209" s="1"/>
+      <c r="BT209" s="1"/>
+      <c r="BU209" s="1"/>
+      <c r="BV209" s="1"/>
+      <c r="BW209" s="1"/>
+      <c r="BX209" s="1"/>
+      <c r="BY209" s="1"/>
+      <c r="BZ209" s="1"/>
+      <c r="CA209" s="1"/>
+      <c r="CB209" s="1"/>
+      <c r="CC209" s="1"/>
+      <c r="CD209" s="1"/>
+      <c r="CE209" s="1"/>
+      <c r="CF209" s="1"/>
+      <c r="CG209" s="1"/>
     </row>
     <row r="210" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A210" s="8"/>
@@ -29333,7 +29365,7 @@
       <c r="CG271" s="2"/>
     </row>
     <row r="272" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A272" s="2"/>
+      <c r="A272" s="8"/>
       <c r="B272" s="2"/>
       <c r="C272" s="3"/>
       <c r="D272" s="2"/>
@@ -30202,6 +30234,93 @@
       <c r="CF281" s="2"/>
       <c r="CG281" s="2"/>
     </row>
+    <row r="282" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A282" s="2"/>
+      <c r="B282" s="2"/>
+      <c r="C282" s="3"/>
+      <c r="D282" s="2"/>
+      <c r="E282" s="2"/>
+      <c r="F282" s="2"/>
+      <c r="G282" s="2"/>
+      <c r="H282" s="2"/>
+      <c r="I282" s="2"/>
+      <c r="J282" s="2"/>
+      <c r="K282" s="2"/>
+      <c r="L282" s="2"/>
+      <c r="M282" s="2"/>
+      <c r="N282" s="2"/>
+      <c r="O282" s="2"/>
+      <c r="P282" s="2"/>
+      <c r="Q282" s="2"/>
+      <c r="R282" s="2"/>
+      <c r="S282" s="2"/>
+      <c r="T282" s="2"/>
+      <c r="U282" s="2"/>
+      <c r="V282" s="2"/>
+      <c r="W282" s="2"/>
+      <c r="X282" s="2"/>
+      <c r="Y282" s="2"/>
+      <c r="Z282" s="2"/>
+      <c r="AA282" s="2"/>
+      <c r="AB282" s="2"/>
+      <c r="AC282" s="2"/>
+      <c r="AD282" s="2"/>
+      <c r="AE282" s="2"/>
+      <c r="AF282" s="2"/>
+      <c r="AG282" s="2"/>
+      <c r="AH282" s="2"/>
+      <c r="AI282" s="2"/>
+      <c r="AJ282" s="2"/>
+      <c r="AK282" s="2"/>
+      <c r="AL282" s="2"/>
+      <c r="AM282" s="2"/>
+      <c r="AN282" s="2"/>
+      <c r="AO282" s="2"/>
+      <c r="AP282" s="2"/>
+      <c r="AQ282" s="2"/>
+      <c r="AR282" s="2"/>
+      <c r="AS282" s="2"/>
+      <c r="AT282" s="2"/>
+      <c r="AU282" s="2"/>
+      <c r="AV282" s="2"/>
+      <c r="AW282" s="2"/>
+      <c r="AX282" s="2"/>
+      <c r="AY282" s="2"/>
+      <c r="AZ282" s="2"/>
+      <c r="BA282" s="2"/>
+      <c r="BB282" s="2"/>
+      <c r="BC282" s="2"/>
+      <c r="BD282" s="2"/>
+      <c r="BE282" s="2"/>
+      <c r="BF282" s="2"/>
+      <c r="BG282" s="2"/>
+      <c r="BH282" s="2"/>
+      <c r="BI282" s="3"/>
+      <c r="BJ282" s="2"/>
+      <c r="BK282" s="2"/>
+      <c r="BL282" s="2"/>
+      <c r="BM282" s="2"/>
+      <c r="BN282" s="2"/>
+      <c r="BO282" s="2"/>
+      <c r="BP282" s="2"/>
+      <c r="BQ282" s="2"/>
+      <c r="BR282" s="2"/>
+      <c r="BS282" s="2"/>
+      <c r="BT282" s="2"/>
+      <c r="BU282" s="2"/>
+      <c r="BV282" s="2"/>
+      <c r="BW282" s="2"/>
+      <c r="BX282" s="2"/>
+      <c r="BY282" s="2"/>
+      <c r="BZ282" s="2"/>
+      <c r="CA282" s="2"/>
+      <c r="CB282" s="2"/>
+      <c r="CC282" s="2"/>
+      <c r="CD282" s="2"/>
+      <c r="CE282" s="2"/>
+      <c r="CF282" s="2"/>
+      <c r="CG282" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="BM25" r:id="rId1" display="abc@test.com"/>
@@ -30224,7 +30343,7 @@
     <hyperlink ref="C72" r:id="rId18"/>
     <hyperlink ref="C25" r:id="rId19"/>
     <hyperlink ref="C11" r:id="rId20"/>
-    <hyperlink ref="C163" r:id="rId21"/>
+    <hyperlink ref="C164" r:id="rId21"/>
     <hyperlink ref="C78" r:id="rId22"/>
     <hyperlink ref="AU78" r:id="rId23" display="Ankit@12345"/>
     <hyperlink ref="C76" r:id="rId24"/>
@@ -30236,30 +30355,30 @@
     <hyperlink ref="C95" r:id="rId30"/>
     <hyperlink ref="C91" r:id="rId31"/>
     <hyperlink ref="C94" r:id="rId32"/>
-    <hyperlink ref="C145" r:id="rId33"/>
-    <hyperlink ref="D145" r:id="rId34" display="Deepika@1234"/>
-    <hyperlink ref="C155" r:id="rId35"/>
-    <hyperlink ref="C156" r:id="rId36"/>
-    <hyperlink ref="C157" r:id="rId37"/>
-    <hyperlink ref="C158" r:id="rId38"/>
-    <hyperlink ref="C160" r:id="rId39"/>
-    <hyperlink ref="C167" r:id="rId40"/>
-    <hyperlink ref="C169" r:id="rId41"/>
-    <hyperlink ref="C170" r:id="rId42"/>
-    <hyperlink ref="D169" r:id="rId43"/>
-    <hyperlink ref="D170" r:id="rId44"/>
+    <hyperlink ref="C146" r:id="rId33"/>
+    <hyperlink ref="D146" r:id="rId34" display="Deepika@1234"/>
+    <hyperlink ref="C156" r:id="rId35"/>
+    <hyperlink ref="C157" r:id="rId36"/>
+    <hyperlink ref="C158" r:id="rId37"/>
+    <hyperlink ref="C159" r:id="rId38"/>
+    <hyperlink ref="C161" r:id="rId39"/>
+    <hyperlink ref="C168" r:id="rId40"/>
+    <hyperlink ref="C170" r:id="rId41"/>
+    <hyperlink ref="C171" r:id="rId42"/>
+    <hyperlink ref="D170" r:id="rId43"/>
+    <hyperlink ref="D171" r:id="rId44"/>
     <hyperlink ref="C54" r:id="rId45"/>
-    <hyperlink ref="C151" r:id="rId46"/>
-    <hyperlink ref="C152" r:id="rId47"/>
-    <hyperlink ref="C153" r:id="rId48"/>
-    <hyperlink ref="C140" r:id="rId49"/>
-    <hyperlink ref="C141" r:id="rId50"/>
-    <hyperlink ref="AM130" r:id="rId51"/>
-    <hyperlink ref="C161" r:id="rId52"/>
-    <hyperlink ref="C162" r:id="rId53"/>
-    <hyperlink ref="C164" r:id="rId54"/>
-    <hyperlink ref="C165" r:id="rId55"/>
-    <hyperlink ref="C166" r:id="rId56"/>
+    <hyperlink ref="C152" r:id="rId46"/>
+    <hyperlink ref="C153" r:id="rId47"/>
+    <hyperlink ref="C154" r:id="rId48"/>
+    <hyperlink ref="C141" r:id="rId49"/>
+    <hyperlink ref="C142" r:id="rId50"/>
+    <hyperlink ref="AM131" r:id="rId51"/>
+    <hyperlink ref="C162" r:id="rId52"/>
+    <hyperlink ref="C163" r:id="rId53"/>
+    <hyperlink ref="C165" r:id="rId54"/>
+    <hyperlink ref="C166" r:id="rId55"/>
+    <hyperlink ref="C167" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId57"/>

</xml_diff>

<commit_message>
Latest Sprint 16 changes
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15660" windowHeight="6225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="5265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
     <sheet name="Dependencies" sheetId="6" r:id="rId2"/>
     <sheet name="updates" sheetId="7" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
@@ -2007,10 +2007,10 @@
   <dimension ref="A1:CG284"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomRight" activeCell="BP9" sqref="BP9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,7 +3485,9 @@
         <v>48</v>
       </c>
       <c r="BR14" s="1"/>
-      <c r="BS14" s="1"/>
+      <c r="BS14" s="1">
+        <v>6575</v>
+      </c>
       <c r="BT14" s="1"/>
       <c r="BU14" s="1"/>
       <c r="BV14" s="1"/>

</xml_diff>